<commit_message>
changes on excel output file column names'
</commit_message>
<xml_diff>
--- a/ETL/clean_data/proyecto_asistencia.xlsx
+++ b/ETL/clean_data/proyecto_asistencia.xlsx
@@ -463,47 +463,47 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>evento_1</t>
+          <t>fecha 1</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>evento_2</t>
+          <t>fecha 2</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>evento_3</t>
+          <t>fecha 3</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>evento_4</t>
+          <t>fecha 4</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>evento_5</t>
+          <t>fecha 5</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>evento_6</t>
+          <t>fecha 6</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>evento_7</t>
+          <t>fecha 7</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>evento_8</t>
+          <t>fecha 8</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>evento_9</t>
+          <t>fecha 9</t>
         </is>
       </c>
     </row>
@@ -4698,47 +4698,47 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>evento_1</t>
+          <t>fecha 1</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>evento_2</t>
+          <t>fecha 2</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>evento_3</t>
+          <t>fecha 3</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>evento_4</t>
+          <t>fecha 4</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>evento_5</t>
+          <t>fecha 5</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>evento_6</t>
+          <t>fecha 6</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>evento_7</t>
+          <t>fecha 7</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>evento_8</t>
+          <t>fecha 8</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>evento_9</t>
+          <t>fecha 9</t>
         </is>
       </c>
     </row>
@@ -5213,47 +5213,47 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>evento_1</t>
+          <t>fecha 1</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>evento_2</t>
+          <t>fecha 2</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>evento_3</t>
+          <t>fecha 3</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>evento_4</t>
+          <t>fecha 4</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>evento_5</t>
+          <t>fecha 5</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>evento_6</t>
+          <t>fecha 6</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>evento_7</t>
+          <t>fecha 7</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>evento_8</t>
+          <t>fecha 8</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>evento_9</t>
+          <t>fecha 9</t>
         </is>
       </c>
     </row>
@@ -6410,47 +6410,47 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>evento_1</t>
+          <t>fecha 1</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>evento_2</t>
+          <t>fecha 2</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>evento_3</t>
+          <t>fecha 3</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>evento_4</t>
+          <t>fecha 4</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>evento_5</t>
+          <t>fecha 5</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>evento_6</t>
+          <t>fecha 6</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>evento_7</t>
+          <t>fecha 7</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>evento_8</t>
+          <t>fecha 8</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>evento_9</t>
+          <t>fecha 9</t>
         </is>
       </c>
     </row>
@@ -7669,47 +7669,47 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>evento_1</t>
+          <t>fecha 1</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>evento_2</t>
+          <t>fecha 2</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>evento_3</t>
+          <t>fecha 3</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>evento_4</t>
+          <t>fecha 4</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>evento_5</t>
+          <t>fecha 5</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>evento_6</t>
+          <t>fecha 6</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>evento_7</t>
+          <t>fecha 7</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>evento_8</t>
+          <t>fecha 8</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>evento_9</t>
+          <t>fecha 9</t>
         </is>
       </c>
     </row>
@@ -8618,47 +8618,47 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>evento_1</t>
+          <t>fecha 1</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>evento_2</t>
+          <t>fecha 2</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>evento_3</t>
+          <t>fecha 3</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>evento_4</t>
+          <t>fecha 4</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>evento_5</t>
+          <t>fecha 5</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>evento_6</t>
+          <t>fecha 6</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>evento_7</t>
+          <t>fecha 7</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>evento_8</t>
+          <t>fecha 8</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>evento_9</t>
+          <t>fecha 9</t>
         </is>
       </c>
     </row>
@@ -9257,47 +9257,47 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>evento_1</t>
+          <t>fecha 1</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>evento_2</t>
+          <t>fecha 2</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>evento_3</t>
+          <t>fecha 3</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>evento_4</t>
+          <t>fecha 4</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>evento_5</t>
+          <t>fecha 5</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>evento_6</t>
+          <t>fecha 6</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>evento_7</t>
+          <t>fecha 7</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>evento_8</t>
+          <t>fecha 8</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>evento_9</t>
+          <t>fecha 9</t>
         </is>
       </c>
     </row>
@@ -10950,47 +10950,47 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>evento_1</t>
+          <t>fecha 1</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>evento_2</t>
+          <t>fecha 2</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>evento_3</t>
+          <t>fecha 3</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>evento_4</t>
+          <t>fecha 4</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>evento_5</t>
+          <t>fecha 5</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>evento_6</t>
+          <t>fecha 6</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>evento_7</t>
+          <t>fecha 7</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>evento_8</t>
+          <t>fecha 8</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>evento_9</t>
+          <t>fecha 9</t>
         </is>
       </c>
     </row>
@@ -12705,47 +12705,47 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>evento_1</t>
+          <t>fecha 1</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>evento_2</t>
+          <t>fecha 2</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>evento_3</t>
+          <t>fecha 3</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>evento_4</t>
+          <t>fecha 4</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>evento_5</t>
+          <t>fecha 5</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>evento_6</t>
+          <t>fecha 6</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>evento_7</t>
+          <t>fecha 7</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>evento_8</t>
+          <t>fecha 8</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>evento_9</t>
+          <t>fecha 9</t>
         </is>
       </c>
     </row>
@@ -12910,47 +12910,47 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>evento_1</t>
+          <t>fecha 1</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>evento_2</t>
+          <t>fecha 2</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>evento_3</t>
+          <t>fecha 3</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>evento_4</t>
+          <t>fecha 4</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>evento_5</t>
+          <t>fecha 5</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>evento_6</t>
+          <t>fecha 6</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>evento_7</t>
+          <t>fecha 7</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>evento_8</t>
+          <t>fecha 8</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>evento_9</t>
+          <t>fecha 9</t>
         </is>
       </c>
     </row>
@@ -13053,47 +13053,47 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>evento_1</t>
+          <t>fecha 1</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>evento_2</t>
+          <t>fecha 2</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>evento_3</t>
+          <t>fecha 3</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>evento_4</t>
+          <t>fecha 4</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>evento_5</t>
+          <t>fecha 5</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>evento_6</t>
+          <t>fecha 6</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>evento_7</t>
+          <t>fecha 7</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>evento_8</t>
+          <t>fecha 8</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>evento_9</t>
+          <t>fecha 9</t>
         </is>
       </c>
     </row>
@@ -13196,47 +13196,47 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>evento_1</t>
+          <t>fecha 1</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>evento_2</t>
+          <t>fecha 2</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>evento_3</t>
+          <t>fecha 3</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>evento_4</t>
+          <t>fecha 4</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>evento_5</t>
+          <t>fecha 5</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>evento_6</t>
+          <t>fecha 6</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>evento_7</t>
+          <t>fecha 7</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>evento_8</t>
+          <t>fecha 8</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>evento_9</t>
+          <t>fecha 9</t>
         </is>
       </c>
     </row>
@@ -13339,47 +13339,47 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>evento_1</t>
+          <t>fecha 1</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>evento_2</t>
+          <t>fecha 2</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>evento_3</t>
+          <t>fecha 3</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>evento_4</t>
+          <t>fecha 4</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>evento_5</t>
+          <t>fecha 5</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>evento_6</t>
+          <t>fecha 6</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>evento_7</t>
+          <t>fecha 7</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>evento_8</t>
+          <t>fecha 8</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>evento_9</t>
+          <t>fecha 9</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
add another sheet on the excel output about no registered users
</commit_message>
<xml_diff>
--- a/ETL/clean_data/proyecto_asistencia.xlsx
+++ b/ETL/clean_data/proyecto_asistencia.xlsx
@@ -20,6 +20,7 @@
     <sheet name="Comunicaciones Elec" sheetId="11" state="visible" r:id="rId11"/>
     <sheet name="Telemática" sheetId="12" state="visible" r:id="rId12"/>
     <sheet name="Profesionales" sheetId="13" state="visible" r:id="rId13"/>
+    <sheet name="No Registrados" sheetId="14" state="visible" r:id="rId14"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -8586,6 +8587,1349 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G38"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Nombre</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Apellido</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Correo electrónico</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Hora a la que se unió</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Hora a la que salió</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>NombreCompleto</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>duración</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Javier</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Ballesteros</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>javier.ballesteros@uptc.edu.co</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>2023-09-06 10:02:00</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>2023-09-06 10:30:00</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Javier Ballesteros</t>
+        </is>
+      </c>
+      <c r="G2" t="n">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Mónica</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Quevedo</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>moni**********@***.com</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>2023-09-06 09:46:00</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>2023-09-06 11:29:00</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Mónica Quevedo</t>
+        </is>
+      </c>
+      <c r="G3" t="n">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Cristian David</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Saenz Gamboa</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>cristian.saenz01@uptc.edu.co</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>2023-09-06 10:05:00</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>2023-09-06 12:02:00</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Cristian David Saenz Gamboa</t>
+        </is>
+      </c>
+      <c r="G4" t="n">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Telematics</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Uptc</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>telematics@uptc.edu.co</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>2023-09-06 10:03:00</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>2023-09-06 12:08:00</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Telematics Uptc</t>
+        </is>
+      </c>
+      <c r="G5" t="n">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Brayan</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Borda</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>brayan.borda01@uptc.edu.co</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>2023-09-06 10:02:00</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>2023-09-06 12:04:00</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Brayan Borda01</t>
+        </is>
+      </c>
+      <c r="G6" t="n">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Lorena</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Larotta</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>tele*****************@***.com</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>2023-09-06 10:04:00</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>2023-09-06 10:40:00</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Lorena Larotta</t>
+        </is>
+      </c>
+      <c r="G7" t="n">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Santigo</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Rodriguez Villarruel</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>sant*****************@***.com</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>2023-09-06 10:02:00</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>2023-09-06 11:59:00</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Santigo Rodriguez Villarruel</t>
+        </is>
+      </c>
+      <c r="G8" t="n">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Norbey</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Rojas</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>norbey.rojas@uptc.edu.co</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>2023-09-06 10:03:00</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>2023-09-06 12:04:00</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>Norbey Rojas</t>
+        </is>
+      </c>
+      <c r="G9" t="n">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Cristian David</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Saenz Gamboa</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>cristian.saenz01@uptc.edu.co</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>2023-09-06 10:17:00</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>2023-09-06 11:58:00</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>Cristian David Saenz Gamboa</t>
+        </is>
+      </c>
+      <c r="G10" t="n">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Telematics</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Uptc</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>telematics@uptc.edu.co</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>2023-09-06 10:03:00</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>2023-09-06 12:04:00</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>Telematics Uptc</t>
+        </is>
+      </c>
+      <c r="G11" t="n">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>  </t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Nan</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr"/>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>2023-09-06 10:02:00</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>2023-09-06 11:58:00</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>+57 311 *****26</t>
+        </is>
+      </c>
+      <c r="G12" t="n">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Adquisiciones</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Biblioteca</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>adquisiciones.biblioteca@uptc.edu.co</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>2023-09-06 09:57:00</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>2023-09-06 09:57:00</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>Adquisiciones Biblioteca</t>
+        </is>
+      </c>
+      <c r="G13" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Filyp</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Garoch</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>inge********@***.com</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>2023-09-06 10:03:00</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>2023-09-06 11:47:00</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>Filyp Garoch</t>
+        </is>
+      </c>
+      <c r="G14" t="n">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Mónica</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Quevedo</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>moni**********@***.com</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>2023-09-06 10:03:00</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>2023-09-06 11:53:00</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>Mónica Quevedo</t>
+        </is>
+      </c>
+      <c r="G15" t="n">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Norbey</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Rojas</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>norbey.rojas@uptc.edu.co</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>2023-09-06 10:09:00</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>2023-09-06 11:53:00</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>Norbey Rojas</t>
+        </is>
+      </c>
+      <c r="G16" t="n">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Cristian David</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Saenz Gamboa</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>cristian.saenz01@uptc.edu.co</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>2023-09-06 10:09:00</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>2023-09-06 11:39:00</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>Cristian David Saenz Gamboa</t>
+        </is>
+      </c>
+      <c r="G17" t="n">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Filyp</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Garoch</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>inge********@***.com</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>2023-09-06 10:10:00</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>2023-09-06 11:11:00</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>Filyp Garoch</t>
+        </is>
+      </c>
+      <c r="G18" t="n">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Mónica</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Quevedo</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>moni**********@***.com</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>2023-09-06 09:52:00</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>2023-09-06 11:12:00</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>Mónica Quevedo</t>
+        </is>
+      </c>
+      <c r="G19" t="n">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Santigo</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Rodriguez Villarruel</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>sant*****************@***.com</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>2023-09-06 10:07:00</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>2023-09-06 11:12:00</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>Santigo Rodriguez Villarruel</t>
+        </is>
+      </c>
+      <c r="G20" t="n">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Norbey</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Rojas</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>norbey.rojas@uptc.edu.co</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>2023-09-06 10:59:00</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>2023-09-06 11:12:00</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>Norbey Rojas</t>
+        </is>
+      </c>
+      <c r="G21" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Cristian David</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Saenz Gamboa</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>cristian.saenz01@uptc.edu.co</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>2023-09-06 10:08:00</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>2023-09-06 11:12:00</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>Cristian David Saenz Gamboa</t>
+        </is>
+      </c>
+      <c r="G22" t="n">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Sandra</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>García</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>sand*********@***.com</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>2023-09-06 09:59:00</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>2023-09-06 11:56:00</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>Sandra García</t>
+        </is>
+      </c>
+      <c r="G23" t="n">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Orlando</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Medina Castro</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>orlando.medina@uptc.edu.co</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>2023-09-06 10:04:00</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>2023-09-06 11:57:00</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>Orlando Medina Castro</t>
+        </is>
+      </c>
+      <c r="G24" t="n">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Cristian David</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Saenz Gamboa</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>cristian.saenz01@uptc.edu.co</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>2023-09-06 10:09:00</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>2023-09-06 11:17:00</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>Cristian David Saenz Gamboa</t>
+        </is>
+      </c>
+      <c r="G25" t="n">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Alejandro</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Enciso</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>aenc***@***.com</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>2023-09-06 09:58:00</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>2023-09-06 11:55:00</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>Alejandro Enciso</t>
+        </is>
+      </c>
+      <c r="G26" t="n">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Orlando</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Medina Castro</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>orlando.medina@uptc.edu.co</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>2023-09-06 10:10:00</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>2023-09-06 11:56:00</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>Orlando Medina Castro</t>
+        </is>
+      </c>
+      <c r="G27" t="n">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Norbey</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Rojas</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>norbey.rojas@uptc.edu.co</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>2023-09-06 10:57:00</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>2023-09-06 12:00:00</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>Norbey Rojas</t>
+        </is>
+      </c>
+      <c r="G28" t="n">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Cristian David</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Saenz Gamboa</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>cristian.saenz01@uptc.edu.co</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>2023-09-06 10:31:00</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>2023-09-06 11:52:00</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>Cristian David Saenz Gamboa</t>
+        </is>
+      </c>
+      <c r="G29" t="n">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>  </t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Nan</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr"/>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>2023-09-06 10:20:00</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>2023-09-06 10:21:00</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>+57 311 *****26</t>
+        </is>
+      </c>
+      <c r="G30" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Orlando</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Medina Castro</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>orlando.medina@uptc.edu.co</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>2023-09-06 10:24:00</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>2023-09-06 11:47:00</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>Orlando Medina Castro</t>
+        </is>
+      </c>
+      <c r="G31" t="n">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>Mónica</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Quevedo</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>moni**********@***.com</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>2023-09-06 10:30:00</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>2023-09-06 11:47:00</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>Mónica Quevedo</t>
+        </is>
+      </c>
+      <c r="G32" t="n">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>Monica</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Quevedo Reyes</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>mque******@***.com</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>2023-09-06 09:54:00</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>2023-09-06 10:25:00</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>Monica Quevedo Reyes</t>
+        </is>
+      </c>
+      <c r="G33" t="n">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>Sandra</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>García</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>sand*********@***.com</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>2023-09-06 10:18:00</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>2023-09-06 11:51:00</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>Sandra García</t>
+        </is>
+      </c>
+      <c r="G34" t="n">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>Orlando</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Medina Castro</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>orlando.medina@uptc.edu.co</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>2023-09-06 09:58:00</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>2023-09-06 11:51:00</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>Orlando Medina Castro</t>
+        </is>
+      </c>
+      <c r="G35" t="n">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>Mónica</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>Quevedo</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>moni**********@***.com</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>2023-09-06 09:59:00</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>2023-09-06 11:51:00</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>Mónica Quevedo</t>
+        </is>
+      </c>
+      <c r="G36" t="n">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>Edgar David</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Giraldo Valencia</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>edga*********@***.com</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>2023-09-06 09:55:00</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>2023-09-06 11:26:00</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>Edgar David Giraldo Valencia</t>
+        </is>
+      </c>
+      <c r="G37" t="n">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>Orlando</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>Medina Castro</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>orlando.medina@uptc.edu.co</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>2023-09-06 10:09:00</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>2023-09-06 11:11:00</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>Orlando Medina Castro</t>
+        </is>
+      </c>
+      <c r="G38" t="n">
+        <v>62</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>

</xml_diff>